<commit_message>
Added PDF file of pcb and schematic
</commit_message>
<xml_diff>
--- a/Bill_Of_Materials/ExtraBOM.xlsx
+++ b/Bill_Of_Materials/ExtraBOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/greeniusgenius/Documents/GitHub/TWUSDiySynthKit/Bill_Of_Materials/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B441FB1-F002-4840-9745-FEAA67195210}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58909ACD-A332-4E4F-81D6-61D4F214E686}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="880" windowWidth="36000" windowHeight="20220" xr2:uid="{65417A81-D12A-B34F-9DCC-D6F21BFB7158}"/>
   </bookViews>
@@ -494,18 +494,18 @@
     <v>Powered by Refinitiv</v>
     <v>1.3593</v>
     <v>1.2097</v>
-    <v>2.9999999999999997E-4</v>
-    <v>2.2110000000000001E-4</v>
+    <v>1E-4</v>
+    <v>7.3700000000000002E-5</v>
     <v>USD</v>
     <v>GBP</v>
     <v>1.3579000000000001</v>
     <v>Currency Pair</v>
-    <v>45813.907083333332</v>
+    <v>45813.90834490741</v>
     <v>1.3572</v>
     <v>UK Pound Sterling/US Dollar FX Spot Rate</v>
     <v>1.3575999999999999</v>
     <v>1.3568</v>
-    <v>1.3571</v>
+    <v>1.3569</v>
     <v>GBPUSD</v>
     <v>GBP/USD</v>
   </rv>
@@ -1010,7 +1010,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{229321E1-56C4-EF48-BAED-957E3078A472}">
   <dimension ref="A1:L15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="86" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="86" workbookViewId="0">
       <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updated BOM to account for quantity, added 3D renders and stuff
</commit_message>
<xml_diff>
--- a/Bill_Of_Materials/ExtraBOM.xlsx
+++ b/Bill_Of_Materials/ExtraBOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/greeniusgenius/Documents/GitHub/TWUSDiySynthKit/Bill_Of_Materials/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81822110-E06D-6B46-89CD-B464A03C1A8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BFDEDAD-6FAE-F74C-A6F3-FF9A61B606B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="880" windowWidth="36000" windowHeight="20220" xr2:uid="{65417A81-D12A-B34F-9DCC-D6F21BFB7158}"/>
   </bookViews>
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="61">
   <si>
     <t>Reference</t>
   </si>
@@ -105,12 +105,6 @@
     <t>Link / URL</t>
   </si>
   <si>
-    <t>Price (GBP)</t>
-  </si>
-  <si>
-    <t>Price (USD)</t>
-  </si>
-  <si>
     <t>https://static.rapidonline.com/pdf/65-1400e.pdf</t>
   </si>
   <si>
@@ -240,7 +234,28 @@
     <t>The PCB</t>
   </si>
   <si>
-    <t>Total Price</t>
+    <t>Unit Price (GBP)</t>
+  </si>
+  <si>
+    <t>Unit Price (USD)</t>
+  </si>
+  <si>
+    <t>Quantity Price (GBP)</t>
+  </si>
+  <si>
+    <t>Quantity Price (USD)</t>
+  </si>
+  <si>
+    <t>USB</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>GBP</t>
+  </si>
+  <si>
+    <t>USD</t>
   </si>
 </sst>
 </file>
@@ -296,7 +311,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -305,38 +320,16 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
+      <left style="thin">
         <color indexed="64"/>
       </left>
-      <right/>
-      <top style="medium">
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -346,7 +339,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -355,9 +348,8 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -494,18 +486,18 @@
     <v>Powered by Refinitiv</v>
     <v>1.3593</v>
     <v>1.2097</v>
-    <v>5.0000000000000001E-4</v>
-    <v>3.6850000000000001E-4</v>
+    <v>-4.5999999999999999E-3</v>
+    <v>-3.3900000000000002E-3</v>
     <v>USD</v>
     <v>GBP</v>
-    <v>1.3579000000000001</v>
+    <v>1.3584000000000001</v>
     <v>Currency Pair</v>
-    <v>45813.923645833333</v>
-    <v>1.3572</v>
+    <v>45814.568425925929</v>
+    <v>1.3508</v>
     <v>UK Pound Sterling/US Dollar FX Spot Rate</v>
     <v>1.3575999999999999</v>
     <v>1.3568</v>
-    <v>1.3573</v>
+    <v>1.3522000000000001</v>
     <v>GBPUSD</v>
     <v>GBP/USD</v>
   </rv>
@@ -1008,10 +1000,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{229321E1-56C4-EF48-BAED-957E3078A472}">
-  <dimension ref="A1:L15"/>
+  <dimension ref="A1:M15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="86" workbookViewId="0">
-      <selection activeCell="K15" sqref="A1:K15"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="86" workbookViewId="0">
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1021,9 +1013,14 @@
     <col min="5" max="5" width="85.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="21.83203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="81.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1046,94 +1043,115 @@
         <v>5</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>10</v>
+        <v>53</v>
       </c>
       <c r="I1" s="2" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>11</v>
+        <v>54</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="L1" s="2"/>
+        <v>55</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>41</v>
+      </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B2">
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>8</v>
       </c>
       <c r="E2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F2" t="s">
         <v>7</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="H2" s="3">
         <v>1.75</v>
       </c>
       <c r="I2" s="4" cm="1">
         <f t="array" aca="1" ref="I2" ca="1">_FV(I1,"High")</f>
-        <v>1.3579000000000001</v>
+        <v>1.3584000000000001</v>
       </c>
       <c r="J2" s="5">
         <f ca="1">H2*I2</f>
-        <v>2.376325</v>
-      </c>
-      <c r="K2" t="s">
-        <v>44</v>
+        <v>2.3772000000000002</v>
+      </c>
+      <c r="K2" s="3">
+        <f>H2*B2</f>
+        <v>3.5</v>
+      </c>
+      <c r="L2" s="5">
+        <f ca="1">J2*B2</f>
+        <v>4.7544000000000004</v>
+      </c>
+      <c r="M2" t="s">
+        <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B3">
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F3" t="s">
         <v>7</v>
       </c>
       <c r="G3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="H3" s="3">
         <v>2.57</v>
       </c>
       <c r="I3" s="4" cm="1">
         <f t="array" aca="1" ref="I3" ca="1">_FV($I$1,"High")</f>
-        <v>1.3579000000000001</v>
+        <v>1.3584000000000001</v>
       </c>
       <c r="J3" s="5">
         <f t="shared" ref="J3:J11" ca="1" si="0">H3*I3</f>
-        <v>3.4898030000000002</v>
-      </c>
-      <c r="K3" t="s">
-        <v>45</v>
+        <v>3.491088</v>
+      </c>
+      <c r="K3" s="3">
+        <f t="shared" ref="K3:K11" si="1">H3*B3</f>
+        <v>5.14</v>
+      </c>
+      <c r="L3" s="5">
+        <f t="shared" ref="L3:L11" ca="1" si="2">J3*B3</f>
+        <v>6.9821759999999999</v>
+      </c>
+      <c r="M3" t="s">
+        <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -1141,172 +1159,212 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="6" t="s">
-        <v>23</v>
-      </c>
       <c r="E4" s="6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H4" s="3">
         <v>0.75</v>
       </c>
       <c r="I4" s="4" cm="1">
         <f t="array" aca="1" ref="I4" ca="1">_FV($I$1,"High")</f>
-        <v>1.3579000000000001</v>
+        <v>1.3584000000000001</v>
       </c>
       <c r="J4" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>1.0184250000000001</v>
-      </c>
-      <c r="K4" t="s">
-        <v>46</v>
+        <v>1.0188000000000001</v>
+      </c>
+      <c r="K4" s="3">
+        <f t="shared" si="1"/>
+        <v>0.75</v>
+      </c>
+      <c r="L4" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>1.0188000000000001</v>
+      </c>
+      <c r="M4" t="s">
+        <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B5">
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H5" s="3">
         <v>0.81</v>
       </c>
       <c r="I5" s="4" cm="1">
         <f t="array" aca="1" ref="I5" ca="1">_FV($I$1,"High")</f>
-        <v>1.3579000000000001</v>
+        <v>1.3584000000000001</v>
       </c>
       <c r="J5" s="5">
         <f ca="1">H6*I5</f>
-        <v>2.2133769999999999</v>
+        <v>2.2141920000000002</v>
+      </c>
+      <c r="K5" s="3">
+        <f t="shared" si="1"/>
+        <v>0.81</v>
+      </c>
+      <c r="L5" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>2.2141920000000002</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B6">
         <v>1</v>
       </c>
       <c r="C6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" t="s">
         <v>29</v>
       </c>
-      <c r="D6" t="s">
-        <v>31</v>
-      </c>
       <c r="E6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H6" s="3">
         <v>1.63</v>
       </c>
       <c r="I6" s="4" cm="1">
         <f t="array" aca="1" ref="I6" ca="1">_FV($I$1,"High")</f>
-        <v>1.3579000000000001</v>
+        <v>1.3584000000000001</v>
       </c>
       <c r="J6" s="5">
         <f ca="1">H7*I6</f>
-        <v>1.914639</v>
+        <v>1.9153439999999999</v>
+      </c>
+      <c r="K6" s="3">
+        <f t="shared" si="1"/>
+        <v>1.63</v>
+      </c>
+      <c r="L6" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>1.9153439999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B7">
         <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G7" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H7" s="3">
         <v>1.41</v>
       </c>
       <c r="I7" s="4" cm="1">
         <f t="array" aca="1" ref="I7" ca="1">_FV($I$1,"High")</f>
-        <v>1.3579000000000001</v>
+        <v>1.3584000000000001</v>
       </c>
       <c r="J7" s="5">
         <f ca="1">H7*I7</f>
-        <v>1.914639</v>
+        <v>1.9153439999999999</v>
+      </c>
+      <c r="K7" s="3">
+        <f t="shared" si="1"/>
+        <v>2.82</v>
+      </c>
+      <c r="L7" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>3.8306879999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B8">
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F8" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G8" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H8" s="3">
         <v>0.75</v>
       </c>
       <c r="I8" s="4" cm="1">
         <f t="array" aca="1" ref="I8" ca="1">_FV($I$1,"High")</f>
-        <v>1.3579000000000001</v>
+        <v>1.3584000000000001</v>
       </c>
       <c r="J8" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>1.0184250000000001</v>
+        <v>1.0188000000000001</v>
+      </c>
+      <c r="K8" s="3">
+        <f t="shared" si="1"/>
+        <v>0.75</v>
+      </c>
+      <c r="L8" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>1.0188000000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -1314,126 +1372,165 @@
         <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E9" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F9" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G9" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H9" s="3">
         <v>1.26</v>
       </c>
       <c r="I9" s="4" cm="1">
         <f t="array" aca="1" ref="I9" ca="1">_FV($I$1,"High")</f>
-        <v>1.3579000000000001</v>
+        <v>1.3584000000000001</v>
       </c>
       <c r="J9" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>1.7109540000000001</v>
-      </c>
-      <c r="K9" t="s">
-        <v>47</v>
+        <v>1.711584</v>
+      </c>
+      <c r="K9" s="3">
+        <f t="shared" si="1"/>
+        <v>1.26</v>
+      </c>
+      <c r="L9" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>1.711584</v>
+      </c>
+      <c r="M9" t="s">
+        <v>45</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>57</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
       <c r="C10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D10" t="s">
         <v>38</v>
       </c>
-      <c r="D10" t="s">
-        <v>40</v>
-      </c>
       <c r="E10" t="s">
+        <v>37</v>
+      </c>
+      <c r="F10" t="s">
         <v>39</v>
       </c>
-      <c r="F10" t="s">
-        <v>41</v>
-      </c>
       <c r="G10" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H10" s="3">
         <v>3.16</v>
       </c>
       <c r="I10" s="4" cm="1">
         <f t="array" aca="1" ref="I10" ca="1">_FV($I$1,"High")</f>
-        <v>1.3579000000000001</v>
+        <v>1.3584000000000001</v>
       </c>
       <c r="J10" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>4.2909640000000007</v>
-      </c>
-      <c r="K10" t="s">
-        <v>48</v>
+        <v>4.2925440000000004</v>
+      </c>
+      <c r="K10" s="3">
+        <f t="shared" si="1"/>
+        <v>3.16</v>
+      </c>
+      <c r="L10" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>4.2925440000000004</v>
+      </c>
+      <c r="M10" t="s">
+        <v>46</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B11">
         <v>1</v>
       </c>
       <c r="C11" t="s">
+        <v>48</v>
+      </c>
+      <c r="D11" t="s">
+        <v>49</v>
+      </c>
+      <c r="E11" t="s">
         <v>50</v>
       </c>
-      <c r="D11" t="s">
+      <c r="F11" t="s">
         <v>51</v>
       </c>
-      <c r="E11" t="s">
-        <v>52</v>
-      </c>
-      <c r="F11" t="s">
-        <v>53</v>
-      </c>
       <c r="G11" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H11" s="3">
         <v>23.35</v>
       </c>
       <c r="I11" s="4" cm="1">
         <f t="array" aca="1" ref="I11" ca="1">_FV($I$1,"High")</f>
-        <v>1.3579000000000001</v>
+        <v>1.3584000000000001</v>
       </c>
       <c r="J11" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>31.706965000000004</v>
-      </c>
-      <c r="K11" t="s">
-        <v>54</v>
+        <v>31.718640000000004</v>
+      </c>
+      <c r="K11" s="3">
+        <f t="shared" si="1"/>
+        <v>23.35</v>
+      </c>
+      <c r="L11" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>31.718640000000004</v>
+      </c>
+      <c r="M11" t="s">
+        <v>52</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="H12" s="3"/>
       <c r="I12" s="4"/>
       <c r="J12" s="5"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="H13" s="3"/>
       <c r="I13" s="4"/>
       <c r="J13" s="5"/>
     </row>
-    <row r="14" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="G15" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="H15" s="9">
-        <f>SUM(H2:H11)</f>
-        <v>37.44</v>
-      </c>
-      <c r="I15" s="8"/>
-      <c r="J15" s="10">
-        <f ca="1">SUM(J2:J11)</f>
-        <v>51.654516000000001</v>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="K14" t="s">
+        <v>59</v>
+      </c>
+      <c r="L14" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="G15" s="7"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="7"/>
+      <c r="J15" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="K15" s="3">
+        <f>SUM(K2:K12)</f>
+        <v>43.17</v>
+      </c>
+      <c r="L15" s="5">
+        <f ca="1">SUM(L2:L11)</f>
+        <v>59.457167999999996</v>
       </c>
     </row>
   </sheetData>

</xml_diff>